<commit_message>
Uwaga nie dziala ale push leci
</commit_message>
<xml_diff>
--- a/cmake-build-debug/finanse.xlsx
+++ b/cmake-build-debug/finanse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\CLionProjects\Projekt-IO\cmake-build-debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekt-IO\cmake-build-debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A629B5E8-8190-420D-9D42-F2AA110472E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFF6844-5B26-419D-A3CF-DAB8109460C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
+    <workbookView xWindow="5004" yWindow="1296" windowWidth="17280" windowHeight="8964" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,18 +33,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>//</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
     <t>19.01.2023</t>
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>20.01.2023</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>21.01.2023</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -389,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049FB1B4-2A61-4643-8816-8B76EC36FD4B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -416,15 +431,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added final prep work for patient medical history
</commit_message>
<xml_diff>
--- a/cmake-build-debug/finanse.xlsx
+++ b/cmake-build-debug/finanse.xlsx
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>19.01.2023</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -475,6 +481,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>